<commit_message>
updated flap detector spreadsheet
</commit_message>
<xml_diff>
--- a/user_tools/testRunner/flap_detector_results.xlsx
+++ b/user_tools/testRunner/flap_detector_results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="V10_seizures" sheetId="1" state="visible" r:id="rId3"/>
@@ -2685,13 +2685,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="true">
+  <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:N80"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K75" activeCellId="0" sqref="K75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2753,7 +2753,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>6897</v>
       </c>
@@ -2841,7 +2841,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <v>7772</v>
       </c>
@@ -2929,7 +2929,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
         <v>11587</v>
       </c>
@@ -3061,7 +3061,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
         <v>17219</v>
       </c>
@@ -3149,7 +3149,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
         <v>21561</v>
       </c>
@@ -3193,7 +3193,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
         <v>21569</v>
       </c>
@@ -3281,7 +3281,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
         <v>119</v>
       </c>
@@ -3322,7 +3322,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
         <v>31397</v>
       </c>
@@ -3366,7 +3366,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
         <v>31404</v>
       </c>
@@ -3586,7 +3586,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
         <v>115</v>
       </c>
@@ -3630,7 +3630,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
         <v>31402</v>
       </c>
@@ -3674,7 +3674,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
         <v>36812</v>
       </c>
@@ -3718,7 +3718,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
         <v>36799</v>
       </c>
@@ -3762,7 +3762,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
         <v>36872</v>
       </c>
@@ -3850,7 +3850,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
         <v>42147</v>
       </c>
@@ -3894,7 +3894,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
         <v>44115</v>
       </c>
@@ -4026,7 +4026,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
         <v>45781</v>
       </c>
@@ -4070,7 +4070,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
         <v>45795</v>
       </c>
@@ -4114,7 +4114,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
         <v>45800</v>
       </c>
@@ -4334,7 +4334,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="n">
         <v>77999</v>
       </c>
@@ -4375,7 +4375,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="n">
         <v>78001</v>
       </c>
@@ -4416,7 +4416,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="n">
         <v>82313</v>
       </c>
@@ -4460,7 +4460,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="n">
         <v>86357</v>
       </c>
@@ -4504,7 +4504,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="n">
         <v>86656</v>
       </c>
@@ -4548,7 +4548,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="n">
         <v>86657</v>
       </c>
@@ -4636,7 +4636,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="n">
         <v>89428</v>
       </c>
@@ -4768,7 +4768,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="n">
         <v>98163</v>
       </c>
@@ -4812,7 +4812,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="n">
         <v>98167</v>
       </c>
@@ -4856,7 +4856,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="n">
         <v>104899</v>
       </c>
@@ -4900,7 +4900,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="n">
         <v>115492</v>
       </c>
@@ -5120,7 +5120,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="n">
         <v>139198</v>
       </c>
@@ -5164,7 +5164,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="n">
         <v>144986</v>
       </c>
@@ -5208,7 +5208,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="n">
         <v>144990</v>
       </c>
@@ -5296,7 +5296,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="n">
         <v>147357</v>
       </c>
@@ -5340,7 +5340,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="n">
         <v>147728</v>
       </c>
@@ -5384,7 +5384,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="n">
         <v>148954</v>
       </c>
@@ -5428,7 +5428,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="n">
         <v>150197</v>
       </c>
@@ -5472,7 +5472,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="n">
         <v>150627</v>
       </c>
@@ -5560,8 +5560,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="67" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
         <v>282</v>
       </c>
@@ -5587,7 +5586,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
         <v>284</v>
       </c>
@@ -5613,7 +5612,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
         <v>285</v>
       </c>
@@ -5652,33 +5651,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N69">
-    <filterColumn colId="13">
-      <filters>
-        <filter val="Partial, kneeling up, left arm flapping"/>
-        <filter val="Partial- left arm flapping"/>
-        <filter val="Partial.  left arm flapping vigorously while kneeling up."/>
-        <filter val="Partial.  left arm large amplitude flapping during manual alarm.   automatic alarm initiated a bit later as amplitude reduced."/>
-        <filter val="Small partial.  got stuck getting out of bed.  on back.  low frequency flapping of left arm before manual alarm raised."/>
-        <filter val="got stuck getting out of bed.  short period of left arm flapping"/>
-        <filter val="kneeling up, snarling, left hand low frequency flapping"/>
-        <filter val="left arm flapping 1 hz"/>
-        <filter val="partial - left arm flapping.  propped up on right arm.   paralysed down left side for a few minutes afterwards"/>
-        <filter val="partial - propped up, left arm flapping"/>
-        <filter val="partial.   arm flapping"/>
-        <filter val="partial.  kneeling up, head turned to left, left arm flapping."/>
-        <filter val="partial.  left arm flapping"/>
-        <filter val="partial.  left arm flapping about 1-2Hz"/>
-        <filter val="partial. sitting up   left arm flapping"/>
-        <filter val="partial. sitting up   left arm flapping.  short one"/>
-        <filter val="quite short as he woke up.  left arm flapping, then trapped under him"/>
-        <filter val="rolled onto back from sleeping.  left arm flapping"/>
-        <filter val="short seizure.  left hand flapping.  rolled him onto his side so data iffy."/>
-        <filter val="sitting up.  low frequency hand flapping.  did not alarm"/>
-        <filter val="standing. going round in circles.  Then sitting down with vigorous flapping of left hand"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:N69"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -5697,8 +5670,8 @@
   </sheetPr>
   <dimension ref="A1:N330"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A59" activeCellId="0" sqref="A59"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B334" activeCellId="0" sqref="B334"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>